<commit_message>
adding backend server.js and nodemon
</commit_message>
<xml_diff>
--- a/references/Dating.xlsx
+++ b/references/Dating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wodah\Documents\.Woda\Projects\Dating\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D167A290-43B6-44B0-BE94-AEC8C03F6C18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50979C5D-B583-46F2-BF56-5CA1976E0731}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="480" windowWidth="20610" windowHeight="14355" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
+    <workbookView xWindow="2445" yWindow="825" windowWidth="20610" windowHeight="14355" activeTab="1" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
@@ -1741,55 +1741,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -3325,8 +3277,8 @@
   </sheetPr>
   <dimension ref="B1:J25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3337,6 +3289,7 @@
     <col min="6" max="6" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21" x14ac:dyDescent="0.25">
@@ -3430,7 +3383,7 @@
       </c>
       <c r="J8" s="1">
         <f ca="1">TODAY()</f>
-        <v>44288</v>
+        <v>44289</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3727,7 +3680,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>I9=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3748,8 +3701,8 @@
   </sheetPr>
   <dimension ref="C3:Q26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4137,8 +4090,8 @@
   </sheetPr>
   <dimension ref="C1:P38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4738,7 +4691,7 @@
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F12" s="1">
         <f ca="1">TODAY()</f>
-        <v>44288</v>
+        <v>44289</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
@@ -4748,7 +4701,7 @@
       </c>
       <c r="F13" s="2">
         <f ca="1">F12+90</f>
-        <v>44378</v>
+        <v>44379</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
@@ -4757,7 +4710,7 @@
       </c>
       <c r="F14" s="1">
         <f ca="1">F12+35</f>
-        <v>44323</v>
+        <v>44324</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
revised folder structure and package json fix
</commit_message>
<xml_diff>
--- a/references/Dating.xlsx
+++ b/references/Dating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wodah\Documents\.Woda\Projects\Dating\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D50D26-F6E3-4D91-A486-EC7C839FB11C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D44E595-3469-47BC-A664-050C1F9ADFDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="285" windowWidth="20610" windowHeight="14355" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
+    <workbookView xWindow="2445" yWindow="825" windowWidth="20610" windowHeight="14355" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="175">
   <si>
     <t>Questionaire</t>
   </si>
@@ -554,6 +554,12 @@
   </si>
   <si>
     <t>check for availabliltiy user experience table</t>
+  </si>
+  <si>
+    <t>Hary</t>
+  </si>
+  <si>
+    <t>Lary</t>
   </si>
 </sst>
 </file>
@@ -4183,7 +4189,7 @@
   <dimension ref="C1:Q38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4229,7 +4235,7 @@
       <c r="G3" s="153" t="s">
         <v>167</v>
       </c>
-      <c r="I3" t="str">
+      <c r="I3" s="10" t="str">
         <f>I2</f>
         <v xml:space="preserve">Unique </v>
       </c>
@@ -4246,18 +4252,24 @@
         <v>168</v>
       </c>
       <c r="O4" s="12"/>
-      <c r="P4" s="156"/>
+      <c r="P4" s="156" t="s">
+        <v>126</v>
+      </c>
       <c r="Q4" s="157"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E5" s="34"/>
       <c r="O5" s="12"/>
-      <c r="P5" s="158"/>
+      <c r="P5" s="158" t="s">
+        <v>173</v>
+      </c>
       <c r="Q5" s="159"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O6" s="12"/>
-      <c r="P6" s="158"/>
+      <c r="P6" s="158" t="s">
+        <v>174</v>
+      </c>
       <c r="Q6" s="159"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated workflow and database schema
</commit_message>
<xml_diff>
--- a/references/Dating.xlsx
+++ b/references/Dating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wodah\Documents\.Woda\Projects\Dating\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D44E595-3469-47BC-A664-050C1F9ADFDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D050FEBD-D5A0-4AB7-8D93-E5D3882A535D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="825" windowWidth="20610" windowHeight="14355" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
+    <workbookView xWindow="2910" yWindow="540" windowWidth="22545" windowHeight="14355" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Database!$C$1:$R$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Database!$C$1:$R$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Overview!$C$3:$P$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Plan!$B$1:$H$20</definedName>
   </definedNames>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="171">
   <si>
     <t>Questionaire</t>
   </si>
@@ -544,22 +544,10 @@
     <t>********</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique </t>
-  </si>
-  <si>
-    <t>(forces unique screen names for all users by default)</t>
-  </si>
-  <si>
-    <t>UserName Table</t>
-  </si>
-  <si>
-    <t>check for availabliltiy user experience table</t>
-  </si>
-  <si>
-    <t>Hary</t>
-  </si>
-  <si>
-    <t>Lary</t>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>zip code</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1767,20 +1755,15 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2597,13 +2580,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2650,13 +2633,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2815,7 +2798,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2868,7 +2851,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2921,7 +2904,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2939,112 +2922,6 @@
         <a:xfrm>
           <a:off x="1905000" y="2314575"/>
           <a:ext cx="1752600" cy="3514725"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A96A671-13E6-431C-9DFF-2B157851322E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5848350" y="342900"/>
-          <a:ext cx="3695700" cy="314325"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F6309D6-1C2E-4A4B-8D2A-4C1C91736249}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5876925" y="419100"/>
-          <a:ext cx="3676650" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3375,8 +3252,8 @@
   </sheetPr>
   <dimension ref="B1:J25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3385,7 +3262,7 @@
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3470,7 +3347,7 @@
       <c r="D8" s="130"/>
       <c r="E8" s="130"/>
       <c r="F8" s="147"/>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>44287</v>
       </c>
       <c r="H8" s="138">
@@ -3481,7 +3358,7 @@
       </c>
       <c r="J8" s="1">
         <f ca="1">TODAY()</f>
-        <v>44289</v>
+        <v>44292</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3500,12 +3377,14 @@
       <c r="F9" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>44292</v>
       </c>
-      <c r="H9" s="138"/>
+      <c r="H9" s="138">
+        <v>44292</v>
+      </c>
       <c r="I9">
-        <f ca="1">IF(H9="",IF($J$8&gt;G9,1,0),0)</f>
+        <f>IF(H9="",IF($J$8&gt;G9,1,0),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3523,12 +3402,14 @@
       <c r="F10" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>44292</v>
       </c>
-      <c r="H10" s="55"/>
+      <c r="H10" s="138">
+        <v>44292</v>
+      </c>
       <c r="I10">
-        <f t="shared" ref="I10:I20" ca="1" si="0">IF(H10="",IF($J$8&gt;G10,1,0),0)</f>
+        <f t="shared" ref="I10:I20" si="0">IF(H10="",IF($J$8&gt;G10,1,0),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3546,8 +3427,8 @@
       <c r="F11" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="1">
-        <v>44294</v>
+      <c r="G11" s="2">
+        <v>44296</v>
       </c>
       <c r="H11" s="55"/>
       <c r="I11">
@@ -3571,7 +3452,7 @@
       <c r="F12" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>44296</v>
       </c>
       <c r="H12" s="55"/>
@@ -3594,8 +3475,8 @@
       <c r="F13" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="G13" s="1">
-        <v>44299</v>
+      <c r="G13" s="2">
+        <v>44296</v>
       </c>
       <c r="H13" s="55"/>
       <c r="I13">
@@ -3613,7 +3494,7 @@
       </c>
       <c r="E14" s="95"/>
       <c r="F14" s="96"/>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <v>44301</v>
       </c>
       <c r="H14" s="55"/>
@@ -3636,7 +3517,7 @@
       <c r="F15" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>44301</v>
       </c>
       <c r="H15" s="55"/>
@@ -3657,7 +3538,7 @@
       <c r="F16" s="100" t="s">
         <v>120</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2">
         <v>44301</v>
       </c>
       <c r="H16" s="55"/>
@@ -3680,7 +3561,7 @@
       <c r="F17" s="98" t="s">
         <v>124</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="2">
         <v>44301</v>
       </c>
       <c r="H17" s="55"/>
@@ -3703,7 +3584,7 @@
       <c r="F18" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2">
         <v>44301</v>
       </c>
       <c r="H18" s="55"/>
@@ -3720,7 +3601,7 @@
         <v>161</v>
       </c>
       <c r="F19" s="148"/>
-      <c r="G19" s="1">
+      <c r="G19" s="2">
         <v>44303</v>
       </c>
       <c r="H19" s="141"/>
@@ -3737,10 +3618,10 @@
         <v>162</v>
       </c>
       <c r="F20" s="149"/>
-      <c r="G20" s="150">
+      <c r="G20" s="154">
         <v>44306</v>
       </c>
-      <c r="H20" s="151"/>
+      <c r="H20" s="150"/>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
@@ -4186,10 +4067,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="C1:Q38"/>
+  <dimension ref="C1:S39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4202,12 +4083,12 @@
     <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E2" s="59" t="s">
         <v>151</v>
       </c>
@@ -4217,34 +4098,28 @@
       <c r="G2" t="s">
         <v>126</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="J2" t="s">
-        <v>170</v>
-      </c>
+      <c r="I2" s="10"/>
       <c r="O2" s="12"/>
-      <c r="P2" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="F3" s="152" t="s">
+      <c r="P2" s="155"/>
+      <c r="Q2" s="155"/>
+      <c r="R2" s="155"/>
+      <c r="S2" s="155"/>
+    </row>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="F3" s="151" t="s">
         <v>136</v>
       </c>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="152" t="s">
         <v>167</v>
       </c>
-      <c r="I3" s="10" t="str">
-        <f>I2</f>
-        <v xml:space="preserve">Unique </v>
-      </c>
-      <c r="O3" s="154"/>
-      <c r="P3" s="155" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I3" s="10"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="156"/>
+      <c r="Q3" s="155"/>
+      <c r="R3" s="155"/>
+      <c r="S3" s="155"/>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F4" s="65" t="s">
         <v>48</v>
       </c>
@@ -4252,27 +4127,27 @@
         <v>168</v>
       </c>
       <c r="O4" s="12"/>
-      <c r="P4" s="156" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q4" s="157"/>
-    </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="P4" s="155"/>
+      <c r="Q4" s="155"/>
+      <c r="R4" s="155"/>
+      <c r="S4" s="155"/>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E5" s="34"/>
       <c r="O5" s="12"/>
-      <c r="P5" s="158" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q5" s="159"/>
-    </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="P5" s="155"/>
+      <c r="Q5" s="155"/>
+      <c r="R5" s="155"/>
+      <c r="S5" s="155"/>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="O6" s="12"/>
-      <c r="P6" s="158" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q6" s="159"/>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="155"/>
+      <c r="Q6" s="155"/>
+      <c r="R6" s="155"/>
+      <c r="S6" s="155"/>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E7" s="58" t="s">
         <v>150</v>
       </c>
@@ -4280,10 +4155,12 @@
         <v>137</v>
       </c>
       <c r="O7" s="12"/>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="159"/>
-    </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="P7" s="155"/>
+      <c r="Q7" s="155"/>
+      <c r="R7" s="155"/>
+      <c r="S7" s="155"/>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F8" s="88" t="s">
         <v>51</v>
       </c>
@@ -4295,10 +4172,12 @@
       <c r="L8" s="60"/>
       <c r="M8" s="53"/>
       <c r="O8" s="12"/>
-      <c r="P8" s="158"/>
-      <c r="Q8" s="159"/>
-    </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="155"/>
+      <c r="Q8" s="155"/>
+      <c r="R8" s="155"/>
+      <c r="S8" s="155"/>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F9" s="62" t="s">
         <v>165</v>
       </c>
@@ -4310,10 +4189,12 @@
       <c r="L9" s="12"/>
       <c r="M9" s="55"/>
       <c r="O9" s="12"/>
-      <c r="P9" s="158"/>
-      <c r="Q9" s="159"/>
-    </row>
-    <row r="10" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="155"/>
+      <c r="Q9" s="155"/>
+      <c r="R9" s="155"/>
+      <c r="S9" s="155"/>
+    </row>
+    <row r="10" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="62" t="s">
         <v>49</v>
       </c>
@@ -4329,10 +4210,12 @@
       <c r="L10" s="12"/>
       <c r="M10" s="55"/>
       <c r="O10" s="12"/>
-      <c r="P10" s="158"/>
-      <c r="Q10" s="159"/>
-    </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="P10" s="155"/>
+      <c r="Q10" s="155"/>
+      <c r="R10" s="155"/>
+      <c r="S10" s="155"/>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11" s="118" t="s">
         <v>144</v>
       </c>
@@ -4349,10 +4232,12 @@
       <c r="L11" s="12"/>
       <c r="M11" s="55"/>
       <c r="O11" s="12"/>
-      <c r="P11" s="158"/>
-      <c r="Q11" s="159"/>
-    </row>
-    <row r="12" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P11" s="155"/>
+      <c r="Q11" s="155"/>
+      <c r="R11" s="155"/>
+      <c r="S11" s="155"/>
+    </row>
+    <row r="12" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="119" t="s">
         <v>143</v>
       </c>
@@ -4377,10 +4262,12 @@
       <c r="L12" s="12"/>
       <c r="M12" s="55"/>
       <c r="O12" s="12"/>
-      <c r="P12" s="160"/>
-      <c r="Q12" s="161"/>
-    </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="P12" s="155"/>
+      <c r="Q12" s="155"/>
+      <c r="R12" s="155"/>
+      <c r="S12" s="155"/>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F13" s="62" t="s">
         <v>62</v>
       </c>
@@ -4405,13 +4292,17 @@
       <c r="M13" s="55" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="P13" s="155"/>
+      <c r="Q13" s="155"/>
+      <c r="R13" s="155"/>
+      <c r="S13" s="155"/>
+    </row>
+    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F14" s="62" t="s">
-        <v>118</v>
+        <v>169</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -4419,189 +4310,190 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="55"/>
-    </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="F15" s="63" t="s">
+      <c r="P14" s="155"/>
+      <c r="Q14" s="155"/>
+      <c r="R14" s="155"/>
+      <c r="S14" s="155"/>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="F15" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="55"/>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="F16" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="G16" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="57"/>
-    </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E17" s="50"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="57"/>
     </row>
     <row r="18" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E18" s="73" t="s">
+      <c r="E18" s="50"/>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E19" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="F18" s="88" t="s">
+      <c r="F19" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="89"/>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F19" s="52" t="s">
+      <c r="G19" s="89"/>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F20" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="60">
+      <c r="G20" s="60">
         <v>20</v>
       </c>
-      <c r="H19" s="60">
+      <c r="H20" s="60">
         <v>25</v>
       </c>
-      <c r="I19" s="69" t="s">
+      <c r="I20" s="69" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F20" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="70" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="21" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F21" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="70" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F22" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="70" t="s">
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="70" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F22" s="56" t="s">
+    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F23" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="71" t="s">
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="71" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F23" s="34"/>
-    </row>
     <row r="24" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E24" s="73" t="s">
+      <c r="F24" s="34"/>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E25" s="73" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F25" s="88" t="s">
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F26" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="89"/>
-      <c r="O25" t="s">
+      <c r="G26" s="89"/>
+      <c r="O26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F26" s="66" t="s">
+    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F27" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="60" t="s">
+      <c r="G27" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="60"/>
-      <c r="I26" s="53"/>
-      <c r="K26" t="s">
+      <c r="H27" s="60"/>
+      <c r="I27" s="53"/>
+      <c r="K27" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F27" s="67" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H27" s="12"/>
-      <c r="I27" s="55"/>
-      <c r="O27" s="51" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="28" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F28" s="67" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="H28" s="12"/>
       <c r="I28" s="55"/>
-      <c r="O28" t="s">
+      <c r="O28" s="51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F29" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="55"/>
+      <c r="O29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F29" s="68"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="57"/>
-      <c r="O29" t="s">
+    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F30" s="68"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="57"/>
+      <c r="O30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E31" s="74" t="s">
+    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="F31" s="114" t="s">
+      <c r="F32" s="114" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
-        <v>85</v>
-      </c>
-      <c r="G32" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" t="s">
-        <v>71</v>
-      </c>
-      <c r="I32" t="b">
-        <v>0</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G33" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" t="s">
         <v>71</v>
       </c>
       <c r="I33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="G34" s="10" t="b">
         <v>0</v>
@@ -4609,19 +4501,32 @@
       <c r="H34" t="s">
         <v>71</v>
       </c>
-      <c r="I34" s="90" t="b">
+      <c r="I34" t="b">
         <v>1</v>
       </c>
       <c r="J34" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>131</v>
+      </c>
+      <c r="G35" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35" s="90" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E35" s="113"/>
-      <c r="F35" s="37"/>
-    </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E36" s="37"/>
+      <c r="E36" s="113"/>
       <c r="F36" s="37"/>
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
@@ -4631,6 +4536,10 @@
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" s="37"/>
       <c r="F38" s="37"/>
+    </row>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4820,7 +4729,7 @@
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F12" s="1">
         <f ca="1">TODAY()</f>
-        <v>44289</v>
+        <v>44292</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
@@ -4830,7 +4739,7 @@
       </c>
       <c r="F13" s="2">
         <f ca="1">F12+90</f>
-        <v>44379</v>
+        <v>44382</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
@@ -4839,7 +4748,7 @@
       </c>
       <c r="F14" s="1">
         <f ca="1">F12+35</f>
-        <v>44324</v>
+        <v>44327</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated work plan vs target file for 4-6-2021
</commit_message>
<xml_diff>
--- a/references/Dating.xlsx
+++ b/references/Dating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wodah\Documents\.Woda\Projects\Dating\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D050FEBD-D5A0-4AB7-8D93-E5D3882A535D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F51E6D-6249-471B-ABF2-0D809196C4C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="540" windowWidth="22545" windowHeight="14355" activeTab="2" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
+    <workbookView xWindow="2910" yWindow="540" windowWidth="22545" windowHeight="14355" xr2:uid="{78A2A3F8-0A39-47A2-96E5-D1FFE72D8D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="4" r:id="rId1"/>
@@ -557,7 +557,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,8 +636,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -734,6 +740,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="61">
     <border>
@@ -1406,7 +1418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1727,7 +1739,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1764,12 +1775,26 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -3252,8 +3277,8 @@
   </sheetPr>
   <dimension ref="B1:J25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3298,26 +3323,26 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="142"/>
-      <c r="C6" s="143"/>
-      <c r="D6" s="144" t="s">
+      <c r="B6" s="141"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="143" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="144" t="s">
+      <c r="E6" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="144" t="s">
+      <c r="F6" s="143" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="144" t="s">
+      <c r="G6" s="143" t="s">
         <v>153</v>
       </c>
-      <c r="H6" s="145" t="s">
+      <c r="H6" s="144" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="139" t="s">
+      <c r="B7" s="138" t="s">
         <v>159</v>
       </c>
       <c r="C7" s="129" t="s">
@@ -3329,7 +3354,7 @@
       <c r="E7" s="129" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="146" t="s">
+      <c r="F7" s="145" t="s">
         <v>95</v>
       </c>
       <c r="G7" s="18" t="s">
@@ -3340,17 +3365,17 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="140"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="129" t="s">
         <v>160</v>
       </c>
       <c r="D8" s="130"/>
       <c r="E8" s="130"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="2">
+      <c r="F8" s="146"/>
+      <c r="G8" s="157">
         <v>44287</v>
       </c>
-      <c r="H8" s="138">
+      <c r="H8" s="156">
         <v>44287</v>
       </c>
       <c r="I8">
@@ -3377,10 +3402,10 @@
       <c r="F9" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="157">
         <v>44292</v>
       </c>
-      <c r="H9" s="138">
+      <c r="H9" s="156">
         <v>44292</v>
       </c>
       <c r="I9">
@@ -3402,10 +3427,10 @@
       <c r="F10" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="157">
         <v>44292</v>
       </c>
-      <c r="H10" s="138">
+      <c r="H10" s="156">
         <v>44292</v>
       </c>
       <c r="I10">
@@ -3600,11 +3625,11 @@
       <c r="E19" s="133" t="s">
         <v>161</v>
       </c>
-      <c r="F19" s="148"/>
+      <c r="F19" s="147"/>
       <c r="G19" s="2">
         <v>44303</v>
       </c>
-      <c r="H19" s="141"/>
+      <c r="H19" s="140"/>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
@@ -3617,11 +3642,11 @@
       <c r="E20" s="136" t="s">
         <v>162</v>
       </c>
-      <c r="F20" s="149"/>
-      <c r="G20" s="154">
+      <c r="F20" s="148"/>
+      <c r="G20" s="153">
         <v>44306</v>
       </c>
-      <c r="H20" s="150"/>
+      <c r="H20" s="149"/>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
@@ -3659,12 +3684,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>I9=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:G19">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>I10=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4069,7 +4094,7 @@
   </sheetPr>
   <dimension ref="C1:S39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -4100,24 +4125,24 @@
       </c>
       <c r="I2" s="10"/>
       <c r="O2" s="12"/>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="155"/>
-      <c r="R2" s="155"/>
-      <c r="S2" s="155"/>
+      <c r="P2" s="154"/>
+      <c r="Q2" s="154"/>
+      <c r="R2" s="154"/>
+      <c r="S2" s="154"/>
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="F3" s="151" t="s">
+      <c r="F3" s="150" t="s">
         <v>136</v>
       </c>
-      <c r="G3" s="152" t="s">
+      <c r="G3" s="151" t="s">
         <v>167</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="O3" s="153"/>
-      <c r="P3" s="156"/>
-      <c r="Q3" s="155"/>
-      <c r="R3" s="155"/>
-      <c r="S3" s="155"/>
+      <c r="O3" s="152"/>
+      <c r="P3" s="155"/>
+      <c r="Q3" s="154"/>
+      <c r="R3" s="154"/>
+      <c r="S3" s="154"/>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F4" s="65" t="s">
@@ -4127,25 +4152,25 @@
         <v>168</v>
       </c>
       <c r="O4" s="12"/>
-      <c r="P4" s="155"/>
-      <c r="Q4" s="155"/>
-      <c r="R4" s="155"/>
-      <c r="S4" s="155"/>
+      <c r="P4" s="154"/>
+      <c r="Q4" s="154"/>
+      <c r="R4" s="154"/>
+      <c r="S4" s="154"/>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E5" s="34"/>
       <c r="O5" s="12"/>
-      <c r="P5" s="155"/>
-      <c r="Q5" s="155"/>
-      <c r="R5" s="155"/>
-      <c r="S5" s="155"/>
+      <c r="P5" s="154"/>
+      <c r="Q5" s="154"/>
+      <c r="R5" s="154"/>
+      <c r="S5" s="154"/>
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="O6" s="12"/>
-      <c r="P6" s="155"/>
-      <c r="Q6" s="155"/>
-      <c r="R6" s="155"/>
-      <c r="S6" s="155"/>
+      <c r="P6" s="154"/>
+      <c r="Q6" s="154"/>
+      <c r="R6" s="154"/>
+      <c r="S6" s="154"/>
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E7" s="58" t="s">
@@ -4155,10 +4180,10 @@
         <v>137</v>
       </c>
       <c r="O7" s="12"/>
-      <c r="P7" s="155"/>
-      <c r="Q7" s="155"/>
-      <c r="R7" s="155"/>
-      <c r="S7" s="155"/>
+      <c r="P7" s="154"/>
+      <c r="Q7" s="154"/>
+      <c r="R7" s="154"/>
+      <c r="S7" s="154"/>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F8" s="88" t="s">
@@ -4172,10 +4197,10 @@
       <c r="L8" s="60"/>
       <c r="M8" s="53"/>
       <c r="O8" s="12"/>
-      <c r="P8" s="155"/>
-      <c r="Q8" s="155"/>
-      <c r="R8" s="155"/>
-      <c r="S8" s="155"/>
+      <c r="P8" s="154"/>
+      <c r="Q8" s="154"/>
+      <c r="R8" s="154"/>
+      <c r="S8" s="154"/>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F9" s="62" t="s">
@@ -4189,10 +4214,10 @@
       <c r="L9" s="12"/>
       <c r="M9" s="55"/>
       <c r="O9" s="12"/>
-      <c r="P9" s="155"/>
-      <c r="Q9" s="155"/>
-      <c r="R9" s="155"/>
-      <c r="S9" s="155"/>
+      <c r="P9" s="154"/>
+      <c r="Q9" s="154"/>
+      <c r="R9" s="154"/>
+      <c r="S9" s="154"/>
     </row>
     <row r="10" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="62" t="s">
@@ -4210,10 +4235,10 @@
       <c r="L10" s="12"/>
       <c r="M10" s="55"/>
       <c r="O10" s="12"/>
-      <c r="P10" s="155"/>
-      <c r="Q10" s="155"/>
-      <c r="R10" s="155"/>
-      <c r="S10" s="155"/>
+      <c r="P10" s="154"/>
+      <c r="Q10" s="154"/>
+      <c r="R10" s="154"/>
+      <c r="S10" s="154"/>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11" s="118" t="s">
@@ -4232,10 +4257,10 @@
       <c r="L11" s="12"/>
       <c r="M11" s="55"/>
       <c r="O11" s="12"/>
-      <c r="P11" s="155"/>
-      <c r="Q11" s="155"/>
-      <c r="R11" s="155"/>
-      <c r="S11" s="155"/>
+      <c r="P11" s="154"/>
+      <c r="Q11" s="154"/>
+      <c r="R11" s="154"/>
+      <c r="S11" s="154"/>
     </row>
     <row r="12" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="119" t="s">
@@ -4262,10 +4287,10 @@
       <c r="L12" s="12"/>
       <c r="M12" s="55"/>
       <c r="O12" s="12"/>
-      <c r="P12" s="155"/>
-      <c r="Q12" s="155"/>
-      <c r="R12" s="155"/>
-      <c r="S12" s="155"/>
+      <c r="P12" s="154"/>
+      <c r="Q12" s="154"/>
+      <c r="R12" s="154"/>
+      <c r="S12" s="154"/>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F13" s="62" t="s">
@@ -4292,10 +4317,10 @@
       <c r="M13" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="P13" s="155"/>
-      <c r="Q13" s="155"/>
-      <c r="R13" s="155"/>
-      <c r="S13" s="155"/>
+      <c r="P13" s="154"/>
+      <c r="Q13" s="154"/>
+      <c r="R13" s="154"/>
+      <c r="S13" s="154"/>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F14" s="62" t="s">
@@ -4310,10 +4335,10 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="55"/>
-      <c r="P14" s="155"/>
-      <c r="Q14" s="155"/>
-      <c r="R14" s="155"/>
-      <c r="S14" s="155"/>
+      <c r="P14" s="154"/>
+      <c r="Q14" s="154"/>
+      <c r="R14" s="154"/>
+      <c r="S14" s="154"/>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="F15" s="62" t="s">

</xml_diff>